<commit_message>
Matching OCR with master data
</commit_message>
<xml_diff>
--- a/xls/14048-108-240005162_3.xlsx
+++ b/xls/14048-108-240005162_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,21 @@
           <t>Balance</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Coverage (raw)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MatchScore</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -504,6 +519,21 @@
       <c r="G2" t="inlineStr">
         <is>
           <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ค่าห้องผู้ป่วยปกติ และค่าอาหาร</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -535,6 +565,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ค่าห้องผู้ป่วย ICU และค่าอาหาร</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -564,6 +609,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ชดเชยรายได้ - HB Incentive</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -575,22 +635,37 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>ค่ารักษาพยาบาล</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>50,000.00 Per Disability</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>ค่ารักษาพยาบาลทั่วไป</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>50,000.00 Per Disability</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -622,6 +697,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ค่ายาผู้ป่วยกลับบ้าน</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -633,22 +723,37 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>ค่าแพทย์ผ่าตัดและหัตถการ</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>50,000.00 Per Disability</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>ค่าแพทย์เฝ้าจัดและหัตถการ</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>50,000.00 Per Disability</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -680,6 +785,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>ค่าแพทย์เยี่ยมไข้</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -709,6 +829,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>อุบัติเหตุฉุกเฉิน (ER Accident)</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -738,6 +873,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ค่าแพทย์ที่ปรึกษา กรณีผ่าตัด</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -767,6 +917,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ค่าแพทย์ที่ปรึกษา กรณีไม่ผ่าตัด</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -796,6 +961,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>ค่าวิสัญญีแพทย์</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -825,6 +1005,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ค่าบริการรถพยาบาล</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -854,6 +1049,21 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ค่าห้องผ่าตัดและค่าอุปกรณ์ห้องผ่าตัด</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>